<commit_message>
16.11.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list 15-11-2020.xlsx
+++ b/2020/Others/Price list 15-11-2020.xlsx
@@ -246,9 +246,6 @@
     <t>T130</t>
   </si>
   <si>
-    <t>Last Update(15-11-2020)</t>
-  </si>
-  <si>
     <t>L23i</t>
   </si>
   <si>
@@ -271,6 +268,9 @@
   </si>
   <si>
     <t>V99Plus_SKD</t>
+  </si>
+  <si>
+    <t>Last Update(16-11-2020)</t>
   </si>
 </sst>
 </file>
@@ -612,7 +612,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -633,7 +633,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -839,7 +839,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1940,7 +1940,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2387,7 +2387,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2447,7 +2447,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2464,7 +2464,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2527,7 +2527,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2544,7 +2544,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2604,7 +2604,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2637,7 +2637,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2649,7 +2649,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2927,7 +2927,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2938,7 +2938,7 @@
   <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3001,7 +3001,7 @@
       <c r="D4" s="27"/>
       <c r="E4" s="11"/>
       <c r="F4" s="28" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
@@ -3093,7 +3093,7 @@
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
       <c r="F8" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8" s="7">
         <v>4150</v>
@@ -3329,7 +3329,7 @@
       <c r="D18" s="5"/>
       <c r="E18" s="6"/>
       <c r="F18" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G18" s="7">
         <v>5855</v>
@@ -3352,7 +3352,7 @@
       <c r="D19" s="5"/>
       <c r="E19" s="6"/>
       <c r="F19" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G19" s="7">
         <v>6570</v>
@@ -3526,7 +3526,7 @@
     </row>
     <row r="27" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" s="7">
         <v>1100</v>
@@ -3549,7 +3549,7 @@
     </row>
     <row r="28" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" s="7">
         <v>1030</v>
@@ -3618,7 +3618,7 @@
     </row>
     <row r="31" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" s="7">
         <v>1050</v>
@@ -3629,7 +3629,7 @@
       <c r="D31" s="5"/>
       <c r="E31" s="6"/>
       <c r="F31" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G31" s="7">
         <v>3640</v>
@@ -3687,7 +3687,7 @@
     </row>
     <row r="34" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="7">
         <v>1150</v>

</xml_diff>

<commit_message>
22.11.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list 15-11-2020.xlsx
+++ b/2020/Others/Price list 15-11-2020.xlsx
@@ -273,7 +273,7 @@
     <t>D82</t>
   </si>
   <si>
-    <t>Last Update(19-11-2020)</t>
+    <t>Last Update(22-11-2020)</t>
   </si>
 </sst>
 </file>
@@ -615,7 +615,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -636,7 +636,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -842,7 +842,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1943,7 +1943,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2390,7 +2390,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2450,7 +2450,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2467,7 +2467,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2530,7 +2530,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2547,7 +2547,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2607,7 +2607,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2640,7 +2640,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2652,7 +2652,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2930,7 +2930,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2940,8 +2940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
23.11.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/Others/Price list 15-11-2020.xlsx
+++ b/2020/Others/Price list 15-11-2020.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t>Model</t>
   </si>
@@ -273,7 +273,10 @@
     <t>D82</t>
   </si>
   <si>
-    <t>Last Update(22-11-2020)</t>
+    <t>T92</t>
+  </si>
+  <si>
+    <t>Last Update(23-11-2020)</t>
   </si>
 </sst>
 </file>
@@ -615,7 +618,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -636,7 +639,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -842,7 +845,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1943,7 +1946,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2390,7 +2393,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2450,7 +2453,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2467,7 +2470,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2530,7 +2533,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2547,7 +2550,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2607,7 +2610,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2640,7 +2643,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2652,7 +2655,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2930,7 +2933,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2940,8 +2943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3004,7 +3007,7 @@
       <c r="D4" s="27"/>
       <c r="E4" s="11"/>
       <c r="F4" s="28" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
@@ -3805,13 +3808,13 @@
     </row>
     <row r="39" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B39" s="7">
+        <v>1170</v>
+      </c>
+      <c r="C39" s="7">
         <v>1250</v>
-      </c>
-      <c r="C39" s="7">
-        <v>1350</v>
       </c>
       <c r="D39" s="5"/>
       <c r="E39" s="6"/>
@@ -3828,13 +3831,13 @@
     </row>
     <row r="40" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>4</v>
+        <v>72</v>
       </c>
       <c r="B40" s="7">
-        <v>1370</v>
+        <v>1250</v>
       </c>
       <c r="C40" s="7">
-        <v>1490</v>
+        <v>1350</v>
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="6"/>
@@ -3845,13 +3848,13 @@
     </row>
     <row r="41" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B41" s="7">
-        <v>1220</v>
+        <v>1370</v>
       </c>
       <c r="C41" s="7">
-        <v>1320</v>
+        <v>1490</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="6"/>
@@ -3861,9 +3864,15 @@
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A42" s="8"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
+      <c r="A42" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="7">
+        <v>1220</v>
+      </c>
+      <c r="C42" s="7">
+        <v>1320</v>
+      </c>
       <c r="D42" s="5"/>
       <c r="E42" s="6"/>
       <c r="F42" s="8"/>

</xml_diff>